<commit_message>
rerun of some scenarios
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/01_output_LCOE_overview.xlsx
+++ b/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/01_output_LCOE_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\02_runs_EURO\02_output_prepared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFB1626-8FE7-4D0E-85A8-05E27E0EC74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB1F728-C237-4A24-9398-A2D622239CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="510" windowWidth="14400" windowHeight="9570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOE" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>run_name</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>power_price_10p_down_PV</t>
+  </si>
+  <si>
+    <t>only_PV_supply</t>
+  </si>
+  <si>
+    <t>only_PV_supply_PV</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,6 +779,58 @@
         <v>31574.177729999999</v>
       </c>
       <c r="H11">
+        <v>14.09394457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>278.40065220000002</v>
+      </c>
+      <c r="C12">
+        <v>1538.9369380000001</v>
+      </c>
+      <c r="D12">
+        <v>389849663.30000001</v>
+      </c>
+      <c r="E12">
+        <v>-100014.07429999999</v>
+      </c>
+      <c r="F12">
+        <v>98996.813769999993</v>
+      </c>
+      <c r="G12">
+        <v>17908.97133</v>
+      </c>
+      <c r="H12">
+        <v>14.09394457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13">
+        <v>278.40065220000002</v>
+      </c>
+      <c r="C13">
+        <v>1538.9369380000001</v>
+      </c>
+      <c r="D13">
+        <v>389849663.30000001</v>
+      </c>
+      <c r="E13">
+        <v>-100014.07429999999</v>
+      </c>
+      <c r="F13">
+        <v>98996.813769999993</v>
+      </c>
+      <c r="G13">
+        <v>17908.97133</v>
+      </c>
+      <c r="H13">
         <v>14.09394457</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update constant efficiency run
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/01_output_LCOE_overview.xlsx
+++ b/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/01_output_LCOE_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\02_runs_EURO\02_output_prepared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB1F728-C237-4A24-9398-A2D622239CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B006454-DA4B-4430-AC22-9C078B9F16AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOE" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>run_name</t>
   </si>
@@ -113,16 +113,22 @@
     <t>variance_10p_down_PV</t>
   </si>
   <si>
-    <t>power_price_10p_down</t>
-  </si>
-  <si>
-    <t>power_price_10p_down_PV</t>
-  </si>
-  <si>
     <t>only_PV_supply</t>
   </si>
   <si>
     <t>only_PV_supply_PV</t>
+  </si>
+  <si>
+    <t>power_price_10p_down2</t>
+  </si>
+  <si>
+    <t>power_price_10p_down2_PV</t>
+  </si>
+  <si>
+    <t>power_price_10p_up2</t>
+  </si>
+  <si>
+    <t>power_price_10p_up2_PV</t>
   </si>
 </sst>
 </file>
@@ -487,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,22 +585,22 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>209.04945853016881</v>
+        <v>211.15367350174481</v>
       </c>
       <c r="C4">
-        <v>1155.5789513195441</v>
+        <v>1167.2105840790889</v>
       </c>
       <c r="D4">
         <v>389849663.28835982</v>
       </c>
       <c r="E4">
-        <v>8423697.9698793311</v>
+        <v>8598995.7220645156</v>
       </c>
       <c r="F4">
-        <v>172612.21249352439</v>
+        <v>171722.2661028025</v>
       </c>
       <c r="G4">
-        <v>31226.329898326021</v>
+        <v>31065.334571361269</v>
       </c>
       <c r="H4">
         <v>14.09394456604476</v>
@@ -605,22 +611,22 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>162.78453055728249</v>
+        <v>162.92835448889389</v>
       </c>
       <c r="C5">
-        <v>899.83671058053369</v>
+        <v>900.63173731360803</v>
       </c>
       <c r="D5">
         <v>389849663.28835982</v>
       </c>
       <c r="E5">
-        <v>437806.39162587892</v>
+        <v>317634.6576472001</v>
       </c>
       <c r="F5">
-        <v>172612.21249352439</v>
+        <v>171722.2661028025</v>
       </c>
       <c r="G5">
-        <v>31226.329898326021</v>
+        <v>31065.334571361269</v>
       </c>
       <c r="H5">
         <v>14.09394456604476</v>
@@ -784,7 +790,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12">
         <v>278.40065220000002</v>
@@ -810,7 +816,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>278.40065220000002</v>
@@ -841,10 +847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAD43E8-D9A4-43D1-B69F-515031F74BAC}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,54 +1250,106 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16">
-        <v>205.18167849798351</v>
+        <v>195.40011860000001</v>
       </c>
       <c r="C16">
-        <v>1134.1987228082969</v>
+        <v>1080.128434</v>
       </c>
       <c r="D16">
-        <v>389849663.28835982</v>
+        <v>389849663.30000001</v>
       </c>
       <c r="E16">
-        <v>8308303.5585107747</v>
+        <v>6417661.3890000004</v>
       </c>
       <c r="F16">
-        <v>175303.64021488719</v>
+        <v>174403.4406</v>
       </c>
       <c r="G16">
-        <v>31713.221345406739</v>
+        <v>31550.371159999999</v>
       </c>
       <c r="H16">
-        <v>14.09394456604476</v>
+        <v>14.09394457</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>159.55442120874301</v>
+        <v>160.0091674</v>
       </c>
       <c r="C17">
-        <v>881.98138390388499</v>
+        <v>884.4951198</v>
       </c>
       <c r="D17">
-        <v>389849663.28835982</v>
+        <v>389849663.30000001</v>
       </c>
       <c r="E17">
-        <v>309679.26268567942</v>
+        <v>245357.72959999999</v>
       </c>
       <c r="F17">
-        <v>175303.64021488719</v>
+        <v>174403.4406</v>
       </c>
       <c r="G17">
-        <v>31713.221345406739</v>
+        <v>31550.371159999999</v>
       </c>
       <c r="H17">
-        <v>14.09394456604476</v>
+        <v>14.09394457</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>219.34661209999999</v>
+      </c>
+      <c r="C18">
+        <v>1212.4993280000001</v>
+      </c>
+      <c r="D18">
+        <v>389849663.30000001</v>
+      </c>
+      <c r="E18">
+        <v>10580959.26</v>
+      </c>
+      <c r="F18">
+        <v>174343.93210000001</v>
+      </c>
+      <c r="G18">
+        <v>31539.605800000001</v>
+      </c>
+      <c r="H18">
+        <v>14.09394457</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>161.62197520000001</v>
+      </c>
+      <c r="C19">
+        <v>893.4103629</v>
+      </c>
+      <c r="D19">
+        <v>389849663.30000001</v>
+      </c>
+      <c r="E19">
+        <v>517019.08059999999</v>
+      </c>
+      <c r="F19">
+        <v>174343.93210000001</v>
+      </c>
+      <c r="G19">
+        <v>31539.605800000001</v>
+      </c>
+      <c r="H19">
+        <v>14.09394457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update crisis year run
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/01_output_LCOE_overview.xlsx
+++ b/spine_projects/03_output_data/02_runs_EURO/02_output_prepared/01_output_LCOE_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\02_runs_EURO\02_output_prepared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B006454-DA4B-4430-AC22-9C078B9F16AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C53B9D8-D504-4351-B031-2775861F5B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOE" sheetId="3" r:id="rId1"/>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,16 +637,16 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>208.10523651788779</v>
+        <v>241.6948431289498</v>
       </c>
       <c r="C6">
-        <v>1150.359501862768</v>
+        <v>1336.0353828516941</v>
       </c>
       <c r="D6">
         <v>389849663.28835982</v>
       </c>
       <c r="E6">
-        <v>8684423.218772972</v>
+        <v>14550789.14001311</v>
       </c>
       <c r="F6">
         <v>174648.24727385119</v>
@@ -849,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAD43E8-D9A4-43D1-B69F-515031F74BAC}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A19" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>